<commit_message>
fix impor akun mahasiswa
</commit_message>
<xml_diff>
--- a/public/AkunMahasiswa/TemplateDaftarAkunMahasiswa.xlsx
+++ b/public/AkunMahasiswa/TemplateDaftarAkunMahasiswa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Polstat STIS\Laravel\applications\smkm-git-duta\public\AkunMahasiswa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F73F51EA-0B98-4A32-A5C6-3E3A6A853DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831D6D41-5F50-45A8-A938-B9CA08B84D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{0A5A482C-4977-4C35-8E96-A3B76D5000BF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{0A5A482C-4977-4C35-8E96-A3B76D5000BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
   <si>
     <t>Nama</t>
   </si>
@@ -92,6 +92,48 @@
     <t>Ainul</t>
   </si>
   <si>
+    <t>3D34</t>
+  </si>
+  <si>
+    <t>dst</t>
+  </si>
+  <si>
+    <t>Andika</t>
+  </si>
+  <si>
+    <t>Sabila</t>
+  </si>
+  <si>
+    <t>Fauzan</t>
+  </si>
+  <si>
+    <t>Ajeng</t>
+  </si>
+  <si>
+    <t>Khesya</t>
+  </si>
+  <si>
+    <t>Brigitta</t>
+  </si>
+  <si>
+    <t>999888777@stis.ac.id</t>
+  </si>
+  <si>
+    <t>888777666@stis.ac.id</t>
+  </si>
+  <si>
+    <t>777666555@stis.ac.id</t>
+  </si>
+  <si>
+    <t>666555444@stis.ac.id</t>
+  </si>
+  <si>
+    <t>555444333@stis.ac.id</t>
+  </si>
+  <si>
+    <t>444333222@stis.ac.id</t>
+  </si>
+  <si>
     <t>111222333@stis.ac.id</t>
   </si>
   <si>
@@ -108,19 +150,13 @@
   </si>
   <si>
     <t>777888999@stis.ac.id</t>
-  </si>
-  <si>
-    <t>3D34</t>
-  </si>
-  <si>
-    <t>dst</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +168,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -489,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2042DEC1-4F54-4EE9-A394-9DB6F5B789E6}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -521,13 +563,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B2">
-        <v>111222333</v>
+        <v>999888777</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -538,107 +580,210 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B3">
-        <v>222333444</v>
+        <v>888777666</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B4">
-        <v>333444555</v>
+        <v>777666555</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B5">
-        <v>444555666</v>
+        <v>666555444</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B6">
-        <v>666777888</v>
+        <v>555444333</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B7">
-        <v>777888999</v>
+        <v>444333222</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>111222333</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>222333444</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>333444555</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>444555666</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>666777888</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>777888999</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>